<commit_message>
Changed test point parts. Updated parts list. Adjusted board layout.
</commit_message>
<xml_diff>
--- a/part_order_digikey.xlsx
+++ b/part_order_digikey.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeff/Documents/Programming/git/aero-hardware/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeff/code/circuit-design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4866E451-B7E4-F04A-ACD1-E7EACDEF49AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC68D08-C05E-264A-BB0A-4E910062CDB1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16140" xr2:uid="{BCF70D43-9D55-454D-B575-CF8612AC33B5}"/>
   </bookViews>
@@ -17,9 +17,9 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Western_Aero_2020" localSheetId="0">Sheet1!$C$1:$C$3</definedName>
+    <definedName name="Western_Aero_2020" localSheetId="0">Sheet1!$C$1:$C$4</definedName>
     <definedName name="Western_Aero_2020" localSheetId="1">Sheet2!$A$1:$K$51</definedName>
-    <definedName name="Western_Aero_2020_1" localSheetId="0">Sheet1!$A$1:$C$27</definedName>
+    <definedName name="Western_Aero_2020_1" localSheetId="0">Sheet1!$A$1:$C$26</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="207">
   <si>
     <t>Qty</t>
   </si>
@@ -546,12 +546,6 @@
     <t>3mm Yellow Led</t>
   </si>
   <si>
-    <t>Wirepad</t>
-  </si>
-  <si>
-    <t>Testpoint</t>
-  </si>
-  <si>
     <t>LM7805 5V Voltage Regulator</t>
   </si>
   <si>
@@ -702,7 +696,22 @@
     <t>https://www.digikey.com/product-detail/en/microchip-technology/MIC29302WT/576-1124-ND/771593</t>
   </si>
   <si>
-    <t>Heat Sink</t>
+    <t>Heat Sink for TO220</t>
+  </si>
+  <si>
+    <t>Testpoints</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/panasonic-electronic-components/EEA-GA1E100B/P15798CT-ND/3831165</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/vishay-bc-components/K104K15X7RF5TL2/BC1084CT-ND/286706</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/kemet/C322C334M5U5TA/399-4364-ND/818140</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/ohmite/FA-T220-38E/FA-T220-38E-ND/2416492</t>
   </si>
 </sst>
 </file>
@@ -741,18 +750,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -768,7 +771,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -782,8 +785,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -803,11 +804,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Western Aero 2020" connectionId="1" xr16:uid="{44DE392F-005C-A24C-B13E-9A6FFFCE7939}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Western Aero 2020_1" connectionId="2" xr16:uid="{2C7A1B07-4D68-814F-975D-DCB9BC7358C6}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Western Aero 2020_1" connectionId="2" xr16:uid="{2C7A1B07-4D68-814F-975D-DCB9BC7358C6}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Western Aero 2020" connectionId="1" xr16:uid="{44DE392F-005C-A24C-B13E-9A6FFFCE7939}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1111,10 +1112,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B72682B-8746-3F40-A2FE-94034A063EA4}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1128,7 +1129,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -1137,115 +1138,110 @@
         <v>3</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="3" customFormat="1">
       <c r="A2" t="s">
-        <v>169</v>
-      </c>
-      <c r="B2" s="5">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>156</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="E2" t="s">
-        <v>90</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B3" s="5">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B4" s="5">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E4" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B5" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>151</v>
+        <v>170</v>
       </c>
       <c r="B6" s="5">
-        <v>6</v>
-      </c>
-      <c r="D6" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>178</v>
+      </c>
       <c r="E6" t="s">
-        <v>142</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B7" s="5">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>183</v>
@@ -1253,16 +1249,16 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B9" s="5">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1273,10 +1269,10 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1287,10 +1283,10 @@
         <v>4</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E11" t="s">
         <v>40</v>
@@ -1304,10 +1300,10 @@
         <v>21</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E12" t="s">
         <v>44</v>
@@ -1315,45 +1311,51 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B13" s="5">
         <v>2</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D13" s="8"/>
+        <v>190</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>204</v>
+      </c>
       <c r="E13" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B14" s="5">
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D14" s="8"/>
+        <v>190</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>205</v>
+      </c>
       <c r="E14" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B15" s="5">
         <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D15" s="8"/>
+        <v>190</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>203</v>
+      </c>
       <c r="E15" t="s">
         <v>43</v>
       </c>
@@ -1366,10 +1368,10 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E16" t="s">
         <v>86</v>
@@ -1383,10 +1385,10 @@
         <v>1</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E17" t="s">
         <v>62</v>
@@ -1400,10 +1402,10 @@
         <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>192</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>194</v>
       </c>
       <c r="E18" t="s">
         <v>66</v>
@@ -1417,10 +1419,10 @@
         <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E19" t="s">
         <v>71</v>
@@ -1434,10 +1436,10 @@
         <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E20" t="s">
         <v>83</v>
@@ -1451,10 +1453,10 @@
         <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E21" t="s">
         <v>85</v>
@@ -1462,171 +1464,166 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="B22" s="5">
-        <v>7</v>
-      </c>
-      <c r="D22" s="8"/>
+        <v>1</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E22" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B23" s="5">
         <v>1</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E23" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B24" s="5">
         <v>1</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>155</v>
+      <c r="C24" t="s">
+        <v>46</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="E24" t="s">
-        <v>76</v>
+        <v>186</v>
+      </c>
+      <c r="E24" s="1">
+        <v>7805</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B25" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25" t="s">
         <v>46</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="E25" s="1">
-        <v>7805</v>
+        <v>7806</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>154</v>
+        <v>187</v>
       </c>
       <c r="B26" s="5">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="E26" s="1">
-        <v>7806</v>
+        <v>188</v>
+      </c>
+      <c r="E26" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="B27" s="5">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C27" t="s">
-        <v>22</v>
+        <v>154</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="E27" t="s">
-        <v>21</v>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>172</v>
+      </c>
+      <c r="B28" s="5">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>154</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="E28" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>173</v>
+        <v>201</v>
       </c>
       <c r="B29" s="5">
-        <v>100</v>
-      </c>
-      <c r="C29" t="s">
-        <v>156</v>
+        <v>3</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="E29" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" t="s">
-        <v>174</v>
-      </c>
-      <c r="B30" s="5">
-        <v>2</v>
-      </c>
-      <c r="C30" t="s">
-        <v>156</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="E30" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" t="s">
-        <v>203</v>
-      </c>
-      <c r="B31" s="5">
-        <v>3</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:M27">
-    <sortCondition ref="C2:C27"/>
+  <sortState ref="A3:M26">
+    <sortCondition ref="C3:C26"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{2907AE97-305C-AA4B-A15E-D481F2B1DD43}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{9CB76B23-E210-3246-A92F-1A87321EEB76}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{A6A56DF0-1522-F844-B73C-A17557BBC775}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{BEAB20BE-C3B1-774D-A301-53F718C5A41F}"/>
-    <hyperlink ref="D7" r:id="rId5" xr:uid="{6F64C4C1-E976-8446-94E4-1060639BA722}"/>
-    <hyperlink ref="D8" r:id="rId6" xr:uid="{5535687E-4C1B-E74A-9BA9-A3DE8621E117}"/>
-    <hyperlink ref="D23" r:id="rId7" xr:uid="{748D212A-0DA9-CA44-8C28-C394CE0F45DE}"/>
-    <hyperlink ref="D9" r:id="rId8" xr:uid="{9DEA5CEC-0021-7D45-B80D-7383BBF02D09}"/>
-    <hyperlink ref="D10" r:id="rId9" xr:uid="{DFFC9545-FEAB-BA41-9143-9B58BCEC0467}"/>
-    <hyperlink ref="D24" r:id="rId10" xr:uid="{028A79D3-5CD3-E34E-B028-68FC709261EF}"/>
-    <hyperlink ref="D30" r:id="rId11" xr:uid="{5BCD844D-B9C9-B64E-A0CA-31346C77AEDC}"/>
-    <hyperlink ref="D27" r:id="rId12" xr:uid="{87F60B61-4B4F-004A-8242-9DA0DF6AE8BF}"/>
-    <hyperlink ref="D20" r:id="rId13" xr:uid="{9F973DBF-BBFA-0745-AC5D-D40E7296B965}"/>
-    <hyperlink ref="D18" r:id="rId14" xr:uid="{B1000177-0E6C-6C40-BB8B-B75FD4E315EA}"/>
-    <hyperlink ref="D19" r:id="rId15" xr:uid="{7BF6CED2-91FC-DF48-B1B4-D14AF84B79B1}"/>
-    <hyperlink ref="D17" r:id="rId16" xr:uid="{D9DEDCFD-90DB-2F4E-A568-99AD7EC3DFC1}"/>
-    <hyperlink ref="D21" r:id="rId17" xr:uid="{C848E0C0-355D-FD40-84EA-E1647B6F0B7A}"/>
-    <hyperlink ref="D11" r:id="rId18" xr:uid="{7B884083-E60E-0C4A-A917-4BD74E5FE188}"/>
-    <hyperlink ref="D12" r:id="rId19" xr:uid="{0ADCED4C-1A22-624A-8599-FAD8D090C99D}"/>
-    <hyperlink ref="D29" r:id="rId20" xr:uid="{7EDDCC66-A4C4-B74F-8766-DDF135D13388}"/>
-    <hyperlink ref="D16" r:id="rId21" xr:uid="{E9D360F7-7A1F-EA43-9A8B-9CF9D630E839}"/>
-    <hyperlink ref="D25" r:id="rId22" xr:uid="{1AB1AAF1-1672-744F-877D-7F508E0E061C}"/>
-    <hyperlink ref="D26" r:id="rId23" xr:uid="{69080036-CB88-C74F-9977-BEA4C1240D26}"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{2907AE97-305C-AA4B-A15E-D481F2B1DD43}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{9CB76B23-E210-3246-A92F-1A87321EEB76}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{A6A56DF0-1522-F844-B73C-A17557BBC775}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{BEAB20BE-C3B1-774D-A301-53F718C5A41F}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{5535687E-4C1B-E74A-9BA9-A3DE8621E117}"/>
+    <hyperlink ref="D22" r:id="rId6" xr:uid="{748D212A-0DA9-CA44-8C28-C394CE0F45DE}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{9DEA5CEC-0021-7D45-B80D-7383BBF02D09}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{DFFC9545-FEAB-BA41-9143-9B58BCEC0467}"/>
+    <hyperlink ref="D23" r:id="rId9" xr:uid="{028A79D3-5CD3-E34E-B028-68FC709261EF}"/>
+    <hyperlink ref="D28" r:id="rId10" xr:uid="{5BCD844D-B9C9-B64E-A0CA-31346C77AEDC}"/>
+    <hyperlink ref="D26" r:id="rId11" xr:uid="{87F60B61-4B4F-004A-8242-9DA0DF6AE8BF}"/>
+    <hyperlink ref="D20" r:id="rId12" xr:uid="{9F973DBF-BBFA-0745-AC5D-D40E7296B965}"/>
+    <hyperlink ref="D18" r:id="rId13" xr:uid="{B1000177-0E6C-6C40-BB8B-B75FD4E315EA}"/>
+    <hyperlink ref="D19" r:id="rId14" xr:uid="{7BF6CED2-91FC-DF48-B1B4-D14AF84B79B1}"/>
+    <hyperlink ref="D17" r:id="rId15" xr:uid="{D9DEDCFD-90DB-2F4E-A568-99AD7EC3DFC1}"/>
+    <hyperlink ref="D21" r:id="rId16" xr:uid="{C848E0C0-355D-FD40-84EA-E1647B6F0B7A}"/>
+    <hyperlink ref="D11" r:id="rId17" xr:uid="{7B884083-E60E-0C4A-A917-4BD74E5FE188}"/>
+    <hyperlink ref="D12" r:id="rId18" xr:uid="{0ADCED4C-1A22-624A-8599-FAD8D090C99D}"/>
+    <hyperlink ref="D27" r:id="rId19" xr:uid="{7EDDCC66-A4C4-B74F-8766-DDF135D13388}"/>
+    <hyperlink ref="D16" r:id="rId20" xr:uid="{E9D360F7-7A1F-EA43-9A8B-9CF9D630E839}"/>
+    <hyperlink ref="D24" r:id="rId21" xr:uid="{1AB1AAF1-1672-744F-877D-7F508E0E061C}"/>
+    <hyperlink ref="D25" r:id="rId22" xr:uid="{69080036-CB88-C74F-9977-BEA4C1240D26}"/>
+    <hyperlink ref="D10" r:id="rId23" xr:uid="{D03BCA55-323F-5741-A938-1637AE0FAA27}"/>
+    <hyperlink ref="D15" r:id="rId24" xr:uid="{94E561E3-E9A0-6544-97ED-3673F46D7B1E}"/>
+    <hyperlink ref="D13" r:id="rId25" xr:uid="{22AC92B3-F6A9-C944-A986-191A56B00E9B}"/>
+    <hyperlink ref="D14" r:id="rId26" xr:uid="{A113EBD0-5FBF-A748-A7D5-9EB9121746AF}"/>
+    <hyperlink ref="D29" r:id="rId27" xr:uid="{937A9A7F-4E44-4F4B-B0CE-E9F3C2594F4C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>